<commit_message>
[EDIT] analysen - diagrammiseren
</commit_message>
<xml_diff>
--- a/Documenten/BCLW_analyse.xlsx
+++ b/Documenten/BCLW_analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cees\Documents\RaspberryPi_bclw\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{35B46965-2C8D-40A4-92CD-DDCB7DCE57DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7256E6FC-B199-4354-9971-712F79DC3B03}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="768" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="768" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Naam" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="301">
   <si>
     <t>C1.0 Verwoorden.</t>
   </si>
@@ -3383,6 +3383,15 @@
       </rPr>
       <t>&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>LijnHerkenModel</t>
+  </si>
+  <si>
+    <t>BordHerkenModel</t>
+  </si>
+  <si>
+    <t>Locatie</t>
   </si>
 </sst>
 </file>
@@ -3980,7 +3989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4133,6 +4142,13 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4163,25 +4179,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4199,28 +4215,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4231,6 +4238,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4247,14 +4263,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5271,50 +5283,50 @@
       <c r="B3" s="9"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="86"/>
+      <c r="C4" s="93"/>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="86"/>
+      <c r="C6" s="93"/>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="93"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="87"/>
-      <c r="C9" s="87"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="93" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5333,9 +5345,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:T139"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5398,60 +5412,60 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="96" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
     </row>
     <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="96" t="s">
+      <c r="A8" s="95"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="97"/>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="106"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -5468,24 +5482,24 @@
       <c r="B11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="99"/>
-      <c r="R11" s="99"/>
-      <c r="S11" s="99"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="104"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
-      <c r="Q12" s="99"/>
-      <c r="R12" s="99"/>
-      <c r="S12" s="99"/>
+      <c r="A12" s="103"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
+      <c r="A13" s="103"/>
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="98"/>
-      <c r="R13" s="98"/>
-      <c r="S13" s="98"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -5524,19 +5538,19 @@
       <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="99"/>
-      <c r="S19" s="99"/>
+      <c r="A19" s="103"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="98"/>
+      <c r="A20" s="103"/>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="Q20" s="99"/>
-      <c r="R20" s="99"/>
-      <c r="S20" s="99"/>
+      <c r="Q20" s="104"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="104"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
@@ -5548,17 +5562,1045 @@
       <c r="C21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q21" s="98"/>
-      <c r="R21" s="98"/>
-      <c r="S21" s="98"/>
+      <c r="Q21" s="103"/>
+      <c r="R21" s="103"/>
+      <c r="S21" s="103"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="59" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C32" s="31"/>
+      <c r="D32" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="33"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="34"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>262</v>
+      </c>
+      <c r="H35" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="I35" t="s">
+        <v>261</v>
+      </c>
+      <c r="K35" t="s">
+        <v>286</v>
+      </c>
+      <c r="M35" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="O35" s="55" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" s="51"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="49"/>
+      <c r="D37" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" s="51"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="49"/>
+      <c r="D38" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E38" s="51"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="59" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="30"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="31"/>
+      <c r="D42" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="E42" s="32"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="33"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="34"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>264</v>
+      </c>
+      <c r="H45" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="I45" t="s">
+        <v>261</v>
+      </c>
+      <c r="K45" t="s">
+        <v>288</v>
+      </c>
+      <c r="M45" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="N45" s="91"/>
+      <c r="O45" s="55" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C48" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="59" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="30"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C52" s="31"/>
+      <c r="D52" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="E52" s="32"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C53" s="33"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="34"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>267</v>
+      </c>
+      <c r="J55" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="K55" s="59"/>
+      <c r="M55" t="s">
+        <v>261</v>
+      </c>
+      <c r="O55" t="s">
+        <v>224</v>
+      </c>
+      <c r="R55" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="T55" s="55" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="49"/>
+      <c r="D56" s="132">
+        <v>0.9</v>
+      </c>
+      <c r="E56" s="51"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C57" s="49"/>
+      <c r="D57" s="132">
+        <v>0.85</v>
+      </c>
+      <c r="E57" s="51"/>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C58" s="49"/>
+      <c r="D58" s="132">
+        <v>0.89</v>
+      </c>
+      <c r="E58" s="51"/>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="59" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" s="29"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="30"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C62" s="31"/>
+      <c r="D62" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="E62" s="32"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C63" s="33"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="34"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>269</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="I65" t="s">
+        <v>261</v>
+      </c>
+      <c r="K65" t="s">
+        <v>291</v>
+      </c>
+      <c r="M65" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="N65" s="91"/>
+      <c r="O65" s="55" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="49"/>
+      <c r="D66" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E66" s="51"/>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C67" s="49"/>
+      <c r="D67" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="E67" s="51"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C68" s="49"/>
+      <c r="D68" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E68" s="51"/>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B70" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71" s="29"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="30"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C72" s="31"/>
+      <c r="D72" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="E72" s="32"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C73" s="33"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="34"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>273</v>
+      </c>
+      <c r="H75" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="I75" t="s">
+        <v>261</v>
+      </c>
+      <c r="K75" t="s">
+        <v>293</v>
+      </c>
+      <c r="M75" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="O75" s="55" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" s="49"/>
+      <c r="D76" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E76" s="51"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C77" s="49"/>
+      <c r="D77" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="E77" s="51"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C78" s="49"/>
+      <c r="D78" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E78" s="51"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B80" s="59" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>6</v>
+      </c>
+      <c r="C81" s="29"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="30"/>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C82" s="31"/>
+      <c r="D82" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="E82" s="32"/>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C83" s="33"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="34"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>277</v>
+      </c>
+      <c r="H85" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="I85" t="s">
+        <v>261</v>
+      </c>
+      <c r="K85" t="s">
+        <v>214</v>
+      </c>
+      <c r="M85" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="O85" s="55" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B86" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C86" s="49"/>
+      <c r="D86" s="50">
+        <v>52.358986000000002</v>
+      </c>
+      <c r="E86" s="51"/>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C87" s="49"/>
+      <c r="D87" s="50">
+        <v>38.967449999999999</v>
+      </c>
+      <c r="E87" s="51"/>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C88" s="49"/>
+      <c r="D88" s="50">
+        <v>21.747183</v>
+      </c>
+      <c r="E88" s="51"/>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B90" s="59" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>7</v>
+      </c>
+      <c r="C91" s="29"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="30"/>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C92" s="31"/>
+      <c r="D92" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="E92" s="32"/>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C93" s="33"/>
+      <c r="D93" s="45"/>
+      <c r="E93" s="34"/>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>278</v>
+      </c>
+      <c r="I95" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="J95" s="59"/>
+      <c r="K95" t="s">
+        <v>261</v>
+      </c>
+      <c r="M95" t="s">
+        <v>279</v>
+      </c>
+      <c r="O95" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q95" s="55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B96" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C96" s="49"/>
+      <c r="D96" s="50">
+        <v>4.8851659999999999</v>
+      </c>
+      <c r="E96" s="51"/>
+    </row>
+    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C97" s="49"/>
+      <c r="D97" s="50">
+        <v>125.80132399999999</v>
+      </c>
+      <c r="E97" s="51"/>
+    </row>
+    <row r="98" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C98" s="49"/>
+      <c r="D98" s="50">
+        <v>15.838328000000001</v>
+      </c>
+      <c r="E98" s="51"/>
+    </row>
+    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B100" s="59" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>8</v>
+      </c>
+      <c r="C101" s="29"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="30"/>
+    </row>
+    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C102" s="31"/>
+      <c r="D102" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="E102" s="32"/>
+    </row>
+    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C103" s="33"/>
+      <c r="D103" s="45"/>
+      <c r="E103" s="34"/>
+    </row>
+    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>282</v>
+      </c>
+      <c r="I105" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="J105" s="59"/>
+      <c r="K105" t="s">
+        <v>261</v>
+      </c>
+      <c r="M105" t="s">
+        <v>225</v>
+      </c>
+      <c r="O105" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q105" s="55" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B106" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106" s="49"/>
+      <c r="D106" s="133">
+        <v>0.5</v>
+      </c>
+      <c r="E106" s="51"/>
+    </row>
+    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C107" s="49"/>
+      <c r="D107" s="133">
+        <v>0.3125</v>
+      </c>
+      <c r="E107" s="51"/>
+    </row>
+    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C108" s="49"/>
+      <c r="D108" s="133">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E108" s="51"/>
+    </row>
+    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B111" s="134" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>9</v>
+      </c>
+      <c r="C112" s="29"/>
+      <c r="D112" s="42"/>
+      <c r="E112" s="30"/>
+      <c r="F112" s="29"/>
+      <c r="G112" s="42"/>
+      <c r="H112" s="30"/>
+      <c r="I112" s="29"/>
+      <c r="J112" s="42"/>
+      <c r="K112" s="30"/>
+    </row>
+    <row r="113" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C113" s="31"/>
+      <c r="D113" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="E113" s="32"/>
+      <c r="F113" s="31"/>
+      <c r="G113" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="H113" s="32"/>
+      <c r="I113" s="31"/>
+      <c r="J113" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="K113" s="32"/>
+    </row>
+    <row r="114" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C114" s="33"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="33"/>
+      <c r="G114" s="45"/>
+      <c r="H114" s="34"/>
+      <c r="I114" s="33"/>
+      <c r="J114" s="45"/>
+      <c r="K114" s="34"/>
+    </row>
+    <row r="116" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>192</v>
+      </c>
+      <c r="E116" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="F116" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="H116" t="s">
+        <v>203</v>
+      </c>
+      <c r="K116" t="s">
+        <v>208</v>
+      </c>
+      <c r="L116" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="M116" s="91" t="s">
+        <v>289</v>
+      </c>
+      <c r="N116" t="s">
+        <v>221</v>
+      </c>
+      <c r="O116" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="R116" t="s">
+        <v>212</v>
+      </c>
+      <c r="S116" s="91" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="117" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B117" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C117" s="49"/>
+      <c r="D117" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E117" s="51"/>
+      <c r="F117" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="G117" s="61"/>
+      <c r="H117" s="61"/>
+      <c r="I117" s="49"/>
+      <c r="J117" s="132">
+        <v>0.9</v>
+      </c>
+      <c r="K117" s="51"/>
+    </row>
+    <row r="118" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C118" s="49"/>
+      <c r="D118" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="E118" s="51"/>
+      <c r="F118" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="G118" s="61"/>
+      <c r="H118" s="61"/>
+      <c r="I118" s="49"/>
+      <c r="J118" s="132">
+        <v>0.85</v>
+      </c>
+      <c r="K118" s="51"/>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C119" s="49"/>
+      <c r="D119" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E119" s="51"/>
+      <c r="F119" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="G119" s="61"/>
+      <c r="H119" s="61"/>
+      <c r="I119" s="49"/>
+      <c r="J119" s="132">
+        <v>0.89</v>
+      </c>
+      <c r="K119" s="51"/>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B121" s="134" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="C122" s="29"/>
+      <c r="D122" s="42"/>
+      <c r="E122" s="30"/>
+      <c r="F122" s="29"/>
+      <c r="G122" s="42"/>
+      <c r="H122" s="30"/>
+      <c r="I122" s="29"/>
+      <c r="J122" s="42"/>
+      <c r="K122" s="30"/>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C123" s="31"/>
+      <c r="D123" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="E123" s="32"/>
+      <c r="F123" s="31"/>
+      <c r="G123" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="H123" s="32"/>
+      <c r="I123" s="31"/>
+      <c r="J123" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="K123" s="32"/>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C124" s="33"/>
+      <c r="D124" s="45"/>
+      <c r="E124" s="34"/>
+      <c r="F124" s="33"/>
+      <c r="G124" s="45"/>
+      <c r="H124" s="34"/>
+      <c r="I124" s="33"/>
+      <c r="J124" s="45"/>
+      <c r="K124" s="34"/>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126" t="s">
+        <v>197</v>
+      </c>
+      <c r="E126" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="F126" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="H126" t="s">
+        <v>229</v>
+      </c>
+      <c r="L126" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="M126" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="N126" s="91"/>
+      <c r="O126" t="s">
+        <v>221</v>
+      </c>
+      <c r="P126" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="S126" t="s">
+        <v>212</v>
+      </c>
+      <c r="T126" s="91" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B127" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C127" s="49"/>
+      <c r="D127" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E127" s="51"/>
+      <c r="F127" s="49"/>
+      <c r="G127" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="H127" s="51"/>
+      <c r="I127" s="49"/>
+      <c r="J127" s="132">
+        <v>0.9</v>
+      </c>
+      <c r="K127" s="51"/>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C128" s="49"/>
+      <c r="D128" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="E128" s="51"/>
+      <c r="F128" s="49"/>
+      <c r="G128" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="H128" s="51"/>
+      <c r="I128" s="49"/>
+      <c r="J128" s="132">
+        <v>0.85</v>
+      </c>
+      <c r="K128" s="51"/>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C129" s="49"/>
+      <c r="D129" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E129" s="51"/>
+      <c r="F129" s="49"/>
+      <c r="G129" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="H129" s="51"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="132">
+        <v>0.89</v>
+      </c>
+      <c r="K129" s="51"/>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B131" s="134" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>11</v>
+      </c>
+      <c r="C132" s="29"/>
+      <c r="D132" s="42"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="29"/>
+      <c r="G132" s="42"/>
+      <c r="H132" s="30"/>
+      <c r="I132" s="29"/>
+      <c r="J132" s="42"/>
+      <c r="K132" s="30"/>
+      <c r="L132" s="29"/>
+      <c r="M132" s="42"/>
+      <c r="N132" s="30"/>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C133" s="31"/>
+      <c r="D133" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="E133" s="32"/>
+      <c r="F133" s="31"/>
+      <c r="G133" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="H133" s="32"/>
+      <c r="I133" s="31"/>
+      <c r="J133" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="K133" s="32"/>
+      <c r="L133" s="31"/>
+      <c r="M133" s="91" t="s">
+        <v>297</v>
+      </c>
+      <c r="N133" s="32"/>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C134" s="33"/>
+      <c r="D134" s="45"/>
+      <c r="E134" s="34"/>
+      <c r="F134" s="33"/>
+      <c r="G134" s="45"/>
+      <c r="H134" s="34"/>
+      <c r="I134" s="33"/>
+      <c r="J134" s="45"/>
+      <c r="K134" s="34"/>
+      <c r="L134" s="33"/>
+      <c r="M134" s="45"/>
+      <c r="N134" s="34"/>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="E136" s="91" t="s">
+        <v>294</v>
+      </c>
+      <c r="F136" s="91"/>
+      <c r="G136" t="s">
+        <v>213</v>
+      </c>
+      <c r="H136" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="I136" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="K136" t="s">
+        <v>215</v>
+      </c>
+      <c r="L136" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="N136" s="91" t="s">
+        <v>296</v>
+      </c>
+      <c r="P136" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q136" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="R136" s="91" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B137" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="C137" s="49"/>
+      <c r="D137" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E137" s="51"/>
+      <c r="F137" s="49"/>
+      <c r="G137" s="50">
+        <v>52.358986000000002</v>
+      </c>
+      <c r="H137" s="51"/>
+      <c r="I137" s="49"/>
+      <c r="J137" s="50">
+        <v>4.8851659999999999</v>
+      </c>
+      <c r="K137" s="51"/>
+      <c r="L137" s="49"/>
+      <c r="M137" s="133">
+        <v>0.5</v>
+      </c>
+      <c r="N137" s="51"/>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C138" s="49"/>
+      <c r="D138" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="E138" s="51"/>
+      <c r="F138" s="49"/>
+      <c r="G138" s="50">
+        <v>38.967449999999999</v>
+      </c>
+      <c r="H138" s="51"/>
+      <c r="I138" s="49"/>
+      <c r="J138" s="50">
+        <v>125.80132399999999</v>
+      </c>
+      <c r="K138" s="51"/>
+      <c r="L138" s="49"/>
+      <c r="M138" s="133">
+        <v>0.3125</v>
+      </c>
+      <c r="N138" s="51"/>
+    </row>
+    <row r="139" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C139" s="49"/>
+      <c r="D139" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E139" s="51"/>
+      <c r="F139" s="49"/>
+      <c r="G139" s="50">
+        <v>21.747183</v>
+      </c>
+      <c r="H139" s="51"/>
+      <c r="I139" s="49"/>
+      <c r="J139" s="50">
+        <v>15.838328000000001</v>
+      </c>
+      <c r="K139" s="51"/>
+      <c r="L139" s="49"/>
+      <c r="M139" s="133">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="N139" s="51"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:G8"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="H8:N8"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="Q20:S20"/>
@@ -5566,11 +6608,6 @@
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="Q12:S12"/>
     <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="A6:G8"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="H8:N8"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5642,118 +6679,118 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="103" t="s">
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="104"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
     </row>
     <row r="7" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="105"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="103" t="s">
+      <c r="A7" s="112"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="111" t="s">
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
-      <c r="N9" s="112"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
     </row>
     <row r="11" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="103" t="s">
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="111"/>
     </row>
     <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="103" t="s">
+      <c r="A12" s="112"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
     </row>
     <row r="13" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="105"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="103" t="s">
+      <c r="A13" s="112"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
@@ -5880,18 +6917,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="H13:N13"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="H13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5964,118 +7001,118 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="123" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
     </row>
     <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="115" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103" t="s">
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="111"/>
     </row>
     <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="123" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="103" t="s">
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="124"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="103" t="s">
+      <c r="A11" s="112"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="111"/>
     </row>
     <row r="12" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="103" t="s">
+      <c r="A12" s="112"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="56" t="s">
@@ -6197,18 +7234,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="H10:N10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="H12:N12"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H12:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6281,24 +7318,24 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -6308,127 +7345,127 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="119" t="s">
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127"/>
+      <c r="K9" s="127"/>
+      <c r="L9" s="127"/>
+      <c r="M9" s="127"/>
+      <c r="N9" s="127"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="105"/>
-      <c r="B10" s="106"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="119" t="s">
+      <c r="A10" s="112"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="127"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="122"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="119" t="s">
+      <c r="B12" s="129"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="127"/>
+      <c r="N12" s="127"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="105"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="119" t="s">
+      <c r="A13" s="112"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
-      <c r="M13" s="120"/>
-      <c r="N13" s="120"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
+      <c r="N13" s="127"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="119" t="s">
+      <c r="A14" s="112"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="114"/>
+      <c r="H14" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="127"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="105"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="119" t="s">
+      <c r="A15" s="112"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="127"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -6595,13 +7632,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="H7:N7"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="H15:N15"/>
     <mergeCell ref="A12:G12"/>
@@ -6610,6 +7640,13 @@
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="H14:N14"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="H10:N10"/>
+    <mergeCell ref="H7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6682,24 +7719,24 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
       <c r="Q6" s="66"/>
       <c r="S6" s="67"/>
     </row>
@@ -6711,15 +7748,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
       <c r="Q7" s="66"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -6727,24 +7764,24 @@
       <c r="S8" s="68"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="119" t="s">
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127"/>
+      <c r="K9" s="127"/>
+      <c r="L9" s="127"/>
+      <c r="M9" s="127"/>
+      <c r="N9" s="127"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -6754,15 +7791,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="127"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
@@ -6772,33 +7809,33 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="118" t="s">
+      <c r="H11" s="122" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="91"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="119" t="s">
+      <c r="A12" s="112"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="126" t="s">
         <v>126</v>
       </c>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="127"/>
+      <c r="N12" s="127"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -6808,15 +7845,15 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="118" t="s">
+      <c r="H13" s="122" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
-      <c r="M13" s="120"/>
-      <c r="N13" s="120"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
+      <c r="N13" s="127"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
@@ -6826,15 +7863,15 @@
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="118" t="s">
+      <c r="H14" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="127"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
@@ -6844,15 +7881,15 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="118" t="s">
+      <c r="H15" s="122" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="127"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127"/>
       <c r="T15" s="69"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -6863,15 +7900,15 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="118" t="s">
+      <c r="H16" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="120"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="127"/>
       <c r="T16" s="68"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -6882,15 +7919,15 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="118" t="s">
+      <c r="H17" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="M17" s="120"/>
-      <c r="N17" s="120"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="127"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
@@ -6900,15 +7937,15 @@
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="118" t="s">
+      <c r="H18" s="122" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-      <c r="N18" s="120"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="127"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T19" s="69"/>
@@ -7124,24 +8161,24 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
       <c r="Q6" s="66"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -7152,15 +8189,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
       <c r="Q7" s="66"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -7171,15 +8208,15 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="118" t="s">
+      <c r="H8" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="91"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
       <c r="Q8" s="66"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7190,15 +8227,15 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="118" t="s">
+      <c r="H9" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="91"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="91"/>
-      <c r="L9" s="91"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
       <c r="Q9" s="66"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7209,15 +8246,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
       <c r="Q10" s="66"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7228,15 +8265,15 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="118" t="s">
+      <c r="H11" s="122" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="91"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
       <c r="Q11" s="66"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7247,15 +8284,15 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="118" t="s">
+      <c r="H12" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="91"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="91"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
       <c r="Q12" s="66"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7266,15 +8303,15 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="118" t="s">
+      <c r="H13" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="91"/>
-      <c r="N13" s="91"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
       <c r="Q13" s="66"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7285,15 +8322,15 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="118" t="s">
+      <c r="H14" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
       <c r="Q14" s="66"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7304,15 +8341,15 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="118" t="s">
+      <c r="H15" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
       <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -7539,24 +8576,24 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
       <c r="Q6" s="66"/>
       <c r="R6" s="69"/>
       <c r="S6" s="68"/>
@@ -7570,15 +8607,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
       <c r="Q7" s="66"/>
       <c r="R7" s="69"/>
       <c r="S7" s="68"/>
@@ -7592,15 +8629,15 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="118" t="s">
+      <c r="H8" s="122" t="s">
         <v>148</v>
       </c>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="91"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
       <c r="Q8" s="66"/>
       <c r="R8" s="69"/>
       <c r="S8" s="68"/>
@@ -7614,15 +8651,15 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="118" t="s">
+      <c r="H9" s="122" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="91"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="91"/>
-      <c r="L9" s="91"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
       <c r="Q9" s="66"/>
       <c r="R9" s="69"/>
       <c r="S9" s="68"/>
@@ -7636,15 +8673,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
       <c r="Q10" s="66"/>
       <c r="R10" s="69"/>
       <c r="S10" s="68"/>
@@ -7658,13 +8695,13 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="91"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
       <c r="Q11" s="66"/>
       <c r="R11" s="69"/>
       <c r="S11" s="69"/>
@@ -7678,15 +8715,15 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="118" t="s">
+      <c r="H12" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="91"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="91"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
       <c r="Q12" s="66"/>
       <c r="S12" s="69"/>
     </row>
@@ -7698,15 +8735,15 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="118" t="s">
+      <c r="H13" s="122" t="s">
         <v>152</v>
       </c>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="91"/>
-      <c r="N13" s="91"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
       <c r="Q13" s="66"/>
       <c r="S13" s="69"/>
     </row>
@@ -7718,15 +8755,15 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="118" t="s">
+      <c r="H14" s="122" t="s">
         <v>144</v>
       </c>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
       <c r="Q14" s="66"/>
       <c r="S14" s="69"/>
     </row>
@@ -7738,15 +8775,15 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="118" t="s">
+      <c r="H15" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
       <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -7926,17 +8963,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="H15:N15"/>
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="H8:N8"/>
     <mergeCell ref="H9:N9"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="H15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8340,7 +9377,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8416,24 +9453,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -8471,7 +9508,7 @@
       <c r="Q17" t="s">
         <v>212</v>
       </c>
-      <c r="R17" s="124">
+      <c r="R17" s="86">
         <v>0.9</v>
       </c>
     </row>
@@ -8506,7 +9543,7 @@
       <c r="Q18" t="s">
         <v>212</v>
       </c>
-      <c r="R18" s="124">
+      <c r="R18" s="86">
         <v>0.85</v>
       </c>
     </row>
@@ -8541,7 +9578,7 @@
       <c r="Q19" t="s">
         <v>212</v>
       </c>
-      <c r="R19" s="124">
+      <c r="R19" s="86">
         <v>0.89</v>
       </c>
     </row>
@@ -8576,7 +9613,7 @@
       <c r="Q21" t="s">
         <v>212</v>
       </c>
-      <c r="R21" s="124">
+      <c r="R21" s="86">
         <v>0.9</v>
       </c>
     </row>
@@ -8611,8 +9648,8 @@
       <c r="Q22" t="s">
         <v>212</v>
       </c>
-      <c r="R22" s="124">
-        <v>0.82</v>
+      <c r="R22" s="86">
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
@@ -8646,8 +9683,8 @@
       <c r="Q23" t="s">
         <v>212</v>
       </c>
-      <c r="R23" s="124">
-        <v>0.81</v>
+      <c r="R23" s="86">
+        <v>0.89</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
@@ -8675,7 +9712,7 @@
       <c r="J25" t="s">
         <v>217</v>
       </c>
-      <c r="L25" s="126">
+      <c r="L25" s="88">
         <v>0.5</v>
       </c>
     </row>
@@ -8704,7 +9741,7 @@
       <c r="J26" t="s">
         <v>217</v>
       </c>
-      <c r="L26" s="126">
+      <c r="L26" s="88">
         <v>0.3125</v>
       </c>
     </row>
@@ -8733,7 +9770,7 @@
       <c r="J27" t="s">
         <v>217</v>
       </c>
-      <c r="L27" s="126">
+      <c r="L27" s="88">
         <v>0.86458333333333337</v>
       </c>
     </row>
@@ -8751,7 +9788,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8815,44 +9852,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="90" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -8889,7 +9926,7 @@
       <c r="P17" t="s">
         <v>212</v>
       </c>
-      <c r="Q17" s="125">
+      <c r="Q17" s="87">
         <v>0.9</v>
       </c>
     </row>
@@ -8902,7 +9939,7 @@
       </c>
       <c r="J18" s="61"/>
       <c r="K18" s="61"/>
-      <c r="Q18" s="125">
+      <c r="Q18" s="87">
         <v>0.85</v>
       </c>
     </row>
@@ -8915,7 +9952,7 @@
       </c>
       <c r="J19" s="61"/>
       <c r="K19" s="61"/>
-      <c r="Q19" s="125">
+      <c r="Q19" s="87">
         <v>0.89</v>
       </c>
     </row>
@@ -8948,7 +9985,7 @@
       <c r="P21" t="s">
         <v>212</v>
       </c>
-      <c r="Q21" s="125">
+      <c r="Q21" s="87">
         <v>0.9</v>
       </c>
     </row>
@@ -8956,12 +9993,12 @@
       <c r="C22" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="J22" s="128" t="s">
+      <c r="J22" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="K22" s="128"/>
-      <c r="Q22" s="125">
-        <v>0.82</v>
+      <c r="K22" s="90"/>
+      <c r="Q22" s="87">
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
@@ -8972,8 +10009,8 @@
         <v>202</v>
       </c>
       <c r="K23" s="61"/>
-      <c r="Q23" s="125">
-        <v>0.81</v>
+      <c r="Q23" s="87">
+        <v>0.89</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
@@ -9004,7 +10041,7 @@
       <c r="K25" t="s">
         <v>225</v>
       </c>
-      <c r="L25" s="127">
+      <c r="L25" s="89">
         <v>0.5</v>
       </c>
     </row>
@@ -9018,7 +10055,7 @@
       <c r="I26" s="61">
         <v>125.80132399999999</v>
       </c>
-      <c r="L26" s="127">
+      <c r="L26" s="89">
         <v>0.3125</v>
       </c>
     </row>
@@ -9032,7 +10069,7 @@
       <c r="I27" s="61">
         <v>15.838328000000001</v>
       </c>
-      <c r="L27" s="127">
+      <c r="L27" s="89">
         <v>0.86458333333333337</v>
       </c>
     </row>
@@ -9052,7 +10089,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:O25"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9116,44 +10153,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="90" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -9193,7 +10230,7 @@
       <c r="Q17" t="s">
         <v>212</v>
       </c>
-      <c r="R17" s="125">
+      <c r="R17" s="87">
         <v>0.9</v>
       </c>
     </row>
@@ -9206,7 +10243,7 @@
       </c>
       <c r="K18" s="61"/>
       <c r="L18" s="61"/>
-      <c r="R18" s="125">
+      <c r="R18" s="87">
         <v>0.85</v>
       </c>
     </row>
@@ -9219,7 +10256,7 @@
       </c>
       <c r="K19" s="61"/>
       <c r="L19" s="61"/>
-      <c r="R19" s="125">
+      <c r="R19" s="87">
         <v>0.89</v>
       </c>
     </row>
@@ -9252,7 +10289,7 @@
       <c r="P21" t="s">
         <v>212</v>
       </c>
-      <c r="Q21" s="125">
+      <c r="Q21" s="87">
         <v>0.9</v>
       </c>
     </row>
@@ -9260,12 +10297,12 @@
       <c r="D22" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="J22" s="128" t="s">
+      <c r="J22" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="K22" s="128"/>
-      <c r="Q22" s="125">
-        <v>0.82</v>
+      <c r="K22" s="90"/>
+      <c r="Q22" s="87">
+        <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
@@ -9276,8 +10313,8 @@
         <v>202</v>
       </c>
       <c r="K23" s="61"/>
-      <c r="Q23" s="125">
-        <v>0.81</v>
+      <c r="Q23" s="87">
+        <v>0.89</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
@@ -9311,7 +10348,7 @@
       <c r="L25" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="M25" s="127">
+      <c r="M25" s="89">
         <v>0.5</v>
       </c>
     </row>
@@ -9325,7 +10362,7 @@
       <c r="J26" s="61">
         <v>125.80132399999999</v>
       </c>
-      <c r="M26" s="127">
+      <c r="M26" s="89">
         <v>0.3125</v>
       </c>
     </row>
@@ -9339,7 +10376,7 @@
       <c r="J27" s="61">
         <v>15.838328000000001</v>
       </c>
-      <c r="M27" s="127">
+      <c r="M27" s="89">
         <v>0.86458333333333337</v>
       </c>
     </row>
@@ -9426,24 +10463,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -9533,24 +10570,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -9586,7 +10623,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="130" t="s">
+      <c r="B17" s="92" t="s">
         <v>231</v>
       </c>
       <c r="E17" t="s">
@@ -9594,7 +10631,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="92" t="s">
         <v>230</v>
       </c>
       <c r="F19" t="s">
@@ -9602,7 +10639,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="130" t="s">
+      <c r="B21" s="92" t="s">
         <v>234</v>
       </c>
       <c r="E21" t="s">
@@ -9610,7 +10647,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="130" t="s">
+      <c r="C23" s="92" t="s">
         <v>235</v>
       </c>
       <c r="F23" t="s">
@@ -9618,7 +10655,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="130" t="s">
+      <c r="B25" s="92" t="s">
         <v>239</v>
       </c>
       <c r="E25" t="s">
@@ -9626,7 +10663,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="92" t="s">
         <v>238</v>
       </c>
       <c r="F27" t="s">
@@ -9634,7 +10671,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="130" t="s">
+      <c r="B29" s="92" t="s">
         <v>242</v>
       </c>
       <c r="E29" t="s">
@@ -9642,7 +10679,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="130" t="s">
+      <c r="C31" s="92" t="s">
         <v>243</v>
       </c>
       <c r="F31" t="s">
@@ -9650,7 +10687,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="130" t="s">
+      <c r="B33" s="92" t="s">
         <v>248</v>
       </c>
       <c r="E33" t="s">
@@ -9658,7 +10695,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="130" t="s">
+      <c r="C35" s="92" t="s">
         <v>246</v>
       </c>
       <c r="F35" t="s">
@@ -9666,7 +10703,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="130" t="s">
+      <c r="B37" s="92" t="s">
         <v>250</v>
       </c>
       <c r="E37" t="s">
@@ -9674,7 +10711,7 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="92" t="s">
         <v>250</v>
       </c>
       <c r="F39" t="s">
@@ -9682,7 +10719,7 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="130" t="s">
+      <c r="B41" s="92" t="s">
         <v>254</v>
       </c>
       <c r="E41" t="s">
@@ -9690,7 +10727,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="92" t="s">
         <v>254</v>
       </c>
       <c r="F43" t="s">
@@ -9698,7 +10735,7 @@
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="130" t="s">
+      <c r="B45" s="92" t="s">
         <v>257</v>
       </c>
       <c r="E45" t="s">
@@ -9706,7 +10743,7 @@
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="130" t="s">
+      <c r="C47" s="92" t="s">
         <v>258</v>
       </c>
       <c r="F47" t="s">
@@ -9726,8 +10763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:U45"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45:O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9791,64 +10828,64 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="90" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="90" t="s">
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="91"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -9945,7 +10982,7 @@
       <c r="M25" t="s">
         <v>268</v>
       </c>
-      <c r="O25" s="125">
+      <c r="O25" s="87">
         <v>0.9</v>
       </c>
       <c r="R25" s="55" t="s">
@@ -9955,14 +10992,14 @@
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H26" s="59"/>
       <c r="I26" s="59"/>
-      <c r="O26" s="125">
+      <c r="O26" s="87">
         <v>0.85</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H27" s="59"/>
       <c r="I27" s="59"/>
-      <c r="O27" s="125">
+      <c r="O27" s="87">
         <v>0.89</v>
       </c>
     </row>
@@ -9991,10 +11028,10 @@
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H30" s="59"/>
       <c r="I30" s="59"/>
-      <c r="O30" s="128" t="s">
+      <c r="O30" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="P30" s="128"/>
+      <c r="P30" s="90"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H31" s="59"/>
@@ -10029,10 +11066,10 @@
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H34" s="59"/>
       <c r="I34" s="59"/>
-      <c r="O34" s="128" t="s">
+      <c r="O34" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="P34" s="128"/>
+      <c r="P34" s="90"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H35" s="59"/>
@@ -10126,7 +11163,7 @@
       <c r="M45" t="s">
         <v>283</v>
       </c>
-      <c r="O45" s="127">
+      <c r="O45" s="89">
         <v>0.5</v>
       </c>
       <c r="R45" s="55" t="s">
@@ -10136,14 +11173,14 @@
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H46" s="59"/>
       <c r="I46" s="59"/>
-      <c r="O46" s="127">
+      <c r="O46" s="89">
         <v>0.3125</v>
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="H47" s="59"/>
       <c r="I47" s="59"/>
-      <c r="O47" s="127">
+      <c r="O47" s="89">
         <v>0.86458333333333337</v>
       </c>
     </row>
@@ -10165,8 +11202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10230,44 +11267,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="90" t="s">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
     </row>
     <row r="7" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="90" t="s">
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -10302,20 +11339,19 @@
       <c r="C17" t="s">
         <v>262</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="G17" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="J17" s="59"/>
-      <c r="L17" t="s">
+      <c r="H17" t="s">
         <v>261</v>
       </c>
-      <c r="N17" t="s">
+      <c r="J17" t="s">
         <v>286</v>
       </c>
-      <c r="Q17" s="129" t="s">
+      <c r="L17" s="91" t="s">
         <v>287</v>
       </c>
-      <c r="S17" s="55" t="s">
+      <c r="N17" s="55" t="s">
         <v>263</v>
       </c>
     </row>
@@ -10326,21 +11362,20 @@
       <c r="C18" t="s">
         <v>264</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="G18" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="J18" s="59"/>
-      <c r="L18" t="s">
+      <c r="H18" t="s">
         <v>261</v>
       </c>
-      <c r="N18" t="s">
+      <c r="J18" t="s">
         <v>288</v>
       </c>
-      <c r="Q18" s="129" t="s">
+      <c r="L18" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="R18" s="129"/>
-      <c r="S18" s="55" t="s">
+      <c r="M18" s="91"/>
+      <c r="N18" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -10361,7 +11396,7 @@
       <c r="N19" t="s">
         <v>224</v>
       </c>
-      <c r="Q19" s="129" t="s">
+      <c r="Q19" s="91" t="s">
         <v>290</v>
       </c>
       <c r="S19" s="55" t="s">
@@ -10375,22 +11410,20 @@
       <c r="C20" t="s">
         <v>269</v>
       </c>
-      <c r="I20" s="59" t="s">
+      <c r="G20" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="J20" s="59"/>
-      <c r="L20" t="s">
+      <c r="H20" t="s">
         <v>261</v>
       </c>
-      <c r="N20" t="s">
+      <c r="J20" t="s">
         <v>291</v>
       </c>
-      <c r="P20" s="129"/>
-      <c r="Q20" s="129" t="s">
+      <c r="L20" s="91" t="s">
         <v>292</v>
       </c>
-      <c r="R20" s="129"/>
-      <c r="S20" s="55" t="s">
+      <c r="M20" s="91"/>
+      <c r="N20" s="55" t="s">
         <v>272</v>
       </c>
     </row>
@@ -10401,21 +11434,19 @@
       <c r="C21" t="s">
         <v>273</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="G21" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="J21" s="59"/>
-      <c r="L21" t="s">
+      <c r="H21" t="s">
         <v>261</v>
       </c>
-      <c r="N21" t="s">
+      <c r="J21" t="s">
         <v>293</v>
       </c>
-      <c r="P21" s="129"/>
-      <c r="Q21" s="129" t="s">
+      <c r="L21" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="S21" s="55" t="s">
+      <c r="N21" s="55" t="s">
         <v>275</v>
       </c>
     </row>
@@ -10426,20 +11457,19 @@
       <c r="C22" t="s">
         <v>277</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="G22" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="J22" s="59"/>
-      <c r="L22" t="s">
+      <c r="H22" t="s">
         <v>261</v>
       </c>
-      <c r="N22" t="s">
+      <c r="J22" t="s">
         <v>214</v>
       </c>
-      <c r="Q22" s="129" t="s">
+      <c r="L22" s="91" t="s">
         <v>295</v>
       </c>
-      <c r="S22" s="55" t="s">
+      <c r="N22" s="55" t="s">
         <v>280</v>
       </c>
     </row>
@@ -10450,20 +11480,20 @@
       <c r="C23" t="s">
         <v>278</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="H23" s="59" t="s">
         <v>279</v>
       </c>
-      <c r="J23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" t="s">
+        <v>261</v>
+      </c>
       <c r="L23" t="s">
-        <v>261</v>
-      </c>
-      <c r="N23" t="s">
         <v>279</v>
       </c>
-      <c r="Q23" s="129" t="s">
+      <c r="N23" s="91" t="s">
         <v>296</v>
       </c>
-      <c r="S23" s="55" t="s">
+      <c r="P23" s="55" t="s">
         <v>281</v>
       </c>
     </row>
@@ -10474,21 +11504,20 @@
       <c r="C24" t="s">
         <v>282</v>
       </c>
-      <c r="I24" s="59" t="s">
+      <c r="H24" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="J24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" t="s">
+        <v>261</v>
+      </c>
       <c r="L24" t="s">
-        <v>261</v>
-      </c>
-      <c r="N24" t="s">
         <v>225</v>
       </c>
-      <c r="P24" s="131"/>
-      <c r="Q24" s="129" t="s">
+      <c r="N24" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="S24" s="55" t="s">
+      <c r="P24" s="55" t="s">
         <v>284</v>
       </c>
     </row>
@@ -10502,7 +11531,7 @@
       <c r="D26" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="129" t="s">
+      <c r="E26" s="91" t="s">
         <v>287</v>
       </c>
       <c r="G26" t="s">
@@ -10514,7 +11543,7 @@
       <c r="K26" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="L26" s="129" t="s">
+      <c r="L26" s="91" t="s">
         <v>289</v>
       </c>
       <c r="M26" t="s">
@@ -10526,7 +11555,7 @@
       <c r="Q26" t="s">
         <v>212</v>
       </c>
-      <c r="R26" s="129" t="s">
+      <c r="R26" s="91" t="s">
         <v>290</v>
       </c>
     </row>
@@ -10540,7 +11569,7 @@
       <c r="D27" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="E27" s="129" t="s">
+      <c r="E27" s="91" t="s">
         <v>287</v>
       </c>
       <c r="G27" t="s">
@@ -10549,10 +11578,10 @@
       <c r="K27" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="L27" s="129" t="s">
+      <c r="L27" s="91" t="s">
         <v>292</v>
       </c>
-      <c r="M27" s="129"/>
+      <c r="M27" s="91"/>
       <c r="N27" t="s">
         <v>221</v>
       </c>
@@ -10562,7 +11591,7 @@
       <c r="R27" t="s">
         <v>212</v>
       </c>
-      <c r="S27" s="129" t="s">
+      <c r="S27" s="91" t="s">
         <v>290</v>
       </c>
     </row>
@@ -10573,17 +11602,17 @@
       <c r="C28" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="D28" s="129" t="s">
+      <c r="D28" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="E28" s="129"/>
+      <c r="E28" s="91"/>
       <c r="F28" t="s">
         <v>213</v>
       </c>
       <c r="G28" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="H28" s="129" t="s">
+      <c r="H28" s="91" t="s">
         <v>295</v>
       </c>
       <c r="J28" t="s">
@@ -10592,7 +11621,7 @@
       <c r="K28" s="59" t="s">
         <v>279</v>
       </c>
-      <c r="M28" s="129" t="s">
+      <c r="M28" s="91" t="s">
         <v>296</v>
       </c>
       <c r="O28" t="s">
@@ -10601,7 +11630,7 @@
       <c r="P28" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="Q28" s="129" t="s">
+      <c r="Q28" s="91" t="s">
         <v>297</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[EDIT] analyse - use case
</commit_message>
<xml_diff>
--- a/Documenten/BCLW_analyse.xlsx
+++ b/Documenten/BCLW_analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cees\Documents\RaspberryPi_bclw\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{694A8DD3-956E-47EB-8C5F-92EA3530E8B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1912B323-2C4E-4189-8274-6CD6A526F30F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="768" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="768" firstSheet="17" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Naam" sheetId="2" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="Activiteiten diagram" sheetId="27" r:id="rId26"/>
   </sheets>
   <calcPr calcId="171027" calcMode="manual"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4374,6 +4375,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4404,25 +4410,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4440,19 +4446,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4463,15 +4478,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4488,11 +4494,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5807,6 +5808,61 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>37258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886E87A4-3299-4CCE-AB0D-B40FDF214181}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="514350"/>
+          <a:ext cx="10058400" cy="4714033"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10171,6 +10227,361 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>96365</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6243640-4EC9-4DDE-829D-0B7B0B8C59A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638175" y="485775"/>
+          <a:ext cx="7992590" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>26175</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>513209</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>188521</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC66DCB-B2D3-4660-9D0B-36085C470D92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="635775" y="3883800"/>
+          <a:ext cx="9021434" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>52350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>82040</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>24196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E16969-DA27-4401-8162-0E98427F4F2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="623850" y="7148475"/>
+          <a:ext cx="7992590" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11850</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>88050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>89167</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>59896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A222BC81-FF75-4AE2-AC67-0E53DBB269AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="621450" y="10613175"/>
+          <a:ext cx="8002117" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>18975</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>47550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>86765</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>19396</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C043E5-D2A3-4491-B1D7-0D8C0CD1C2B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628575" y="14001675"/>
+          <a:ext cx="7992590" cy="3019846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>130190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC655D0-7898-465C-8380-0AF600DA9478}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="17459325"/>
+          <a:ext cx="7772400" cy="8435990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23775</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>99975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>480975</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>155832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA2A6BFE-42D2-471F-9E08-77E2CCCA8DD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="633375" y="26246100"/>
+          <a:ext cx="7772400" cy="8628357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10487,50 +10898,50 @@
       <c r="B3" s="9"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="114"/>
+      <c r="C4" s="119"/>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="114"/>
+      <c r="C6" s="119"/>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="115"/>
-      <c r="C7" s="115"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="114"/>
+      <c r="C8" s="119"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="115"/>
-      <c r="C9" s="115"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="120"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="114" t="s">
+      <c r="C11" s="119" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="115"/>
-      <c r="C12" s="115"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -10616,60 +11027,60 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="126" t="s">
+      <c r="A7" s="121"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
     </row>
     <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="116"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="126" t="s">
+      <c r="A8" s="121"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -10686,24 +11097,24 @@
       <c r="B11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="125"/>
-      <c r="R11" s="125"/>
-      <c r="S11" s="125"/>
+      <c r="Q11" s="132"/>
+      <c r="R11" s="132"/>
+      <c r="S11" s="132"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="124"/>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="125"/>
-      <c r="S12" s="125"/>
+      <c r="A12" s="131"/>
+      <c r="Q12" s="132"/>
+      <c r="R12" s="132"/>
+      <c r="S12" s="132"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="124"/>
+      <c r="A13" s="131"/>
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="124"/>
-      <c r="R13" s="124"/>
-      <c r="S13" s="124"/>
+      <c r="Q13" s="131"/>
+      <c r="R13" s="131"/>
+      <c r="S13" s="131"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -10742,19 +11153,19 @@
       <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="124"/>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="125"/>
-      <c r="S19" s="125"/>
+      <c r="A19" s="131"/>
+      <c r="Q19" s="132"/>
+      <c r="R19" s="132"/>
+      <c r="S19" s="132"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
+      <c r="A20" s="131"/>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="125"/>
-      <c r="S20" s="125"/>
+      <c r="Q20" s="132"/>
+      <c r="R20" s="132"/>
+      <c r="S20" s="132"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
@@ -10766,9 +11177,9 @@
       <c r="C21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q21" s="124"/>
-      <c r="R21" s="124"/>
-      <c r="S21" s="124"/>
+      <c r="Q21" s="131"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="131"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -11800,11 +12211,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A6:G8"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="H8:N8"/>
-    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="Q20:S20"/>
@@ -11812,6 +12218,11 @@
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="Q12:S12"/>
     <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="A6:G8"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="H8:N8"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11885,118 +12296,118 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="130"/>
-      <c r="H6" s="131" t="s">
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="137"/>
+      <c r="M6" s="137"/>
+      <c r="N6" s="137"/>
     </row>
     <row r="7" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="131" t="s">
+      <c r="A7" s="138"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="132"/>
-      <c r="L7" s="132"/>
-      <c r="M7" s="132"/>
-      <c r="N7" s="132"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="137"/>
+      <c r="N7" s="137"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="136" t="s">
+      <c r="A9" s="133" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="139" t="s">
+      <c r="B9" s="134"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="140"/>
-      <c r="J9" s="140"/>
-      <c r="K9" s="140"/>
-      <c r="L9" s="140"/>
-      <c r="M9" s="140"/>
-      <c r="N9" s="140"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="145"/>
+      <c r="L9" s="145"/>
+      <c r="M9" s="145"/>
+      <c r="N9" s="145"/>
     </row>
     <row r="11" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="131" t="s">
+      <c r="B11" s="134"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="132"/>
-      <c r="J11" s="132"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
-      <c r="N11" s="132"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="131" t="s">
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-      <c r="K12" s="132"/>
-      <c r="L12" s="132"/>
-      <c r="M12" s="132"/>
-      <c r="N12" s="132"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="137"/>
+      <c r="N12" s="137"/>
     </row>
     <row r="13" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="133"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="131" t="s">
+      <c r="A13" s="138"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="140"/>
+      <c r="H13" s="136" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="132"/>
-      <c r="J13" s="132"/>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
-      <c r="M13" s="132"/>
-      <c r="N13" s="132"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
+      <c r="N13" s="137"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
@@ -14502,18 +14913,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H11:N11"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="H12:N12"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="H13:N13"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14588,118 +14999,118 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="149" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
-      <c r="N7" s="134"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="139"/>
+      <c r="N7" s="139"/>
     </row>
     <row r="9" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="136" t="s">
+      <c r="A9" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="131" t="s">
+      <c r="B9" s="134"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="136" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
-      <c r="K9" s="132"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="132"/>
-      <c r="N9" s="132"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="137"/>
+      <c r="L9" s="137"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="137"/>
     </row>
     <row r="10" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="144" t="s">
+      <c r="A10" s="146" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="145"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="131" t="s">
+      <c r="B10" s="147"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="147"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
-      <c r="K10" s="132"/>
-      <c r="L10" s="132"/>
-      <c r="M10" s="132"/>
-      <c r="N10" s="132"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="137"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="131" t="s">
+      <c r="A11" s="138"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="139"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="136" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="132"/>
-      <c r="J11" s="132"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
-      <c r="N11" s="132"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
     </row>
     <row r="12" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="131" t="s">
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="136" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-      <c r="K12" s="132"/>
-      <c r="L12" s="132"/>
-      <c r="M12" s="132"/>
-      <c r="N12" s="132"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="137"/>
+      <c r="N12" s="137"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="56" t="s">
@@ -16087,18 +16498,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H11:N11"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="H12:N12"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16173,24 +16584,24 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="149" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -16200,127 +16611,127 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="151" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="141" t="s">
+      <c r="A9" s="149" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="117"/>
-      <c r="C9" s="117"/>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="147" t="s">
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="150"/>
+      <c r="H9" s="152" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="153"/>
+      <c r="K9" s="153"/>
+      <c r="L9" s="153"/>
+      <c r="M9" s="153"/>
+      <c r="N9" s="153"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="147" t="s">
+      <c r="A10" s="138"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="152" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="153"/>
+      <c r="K10" s="153"/>
+      <c r="L10" s="153"/>
+      <c r="M10" s="153"/>
+      <c r="N10" s="153"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="149" t="s">
+      <c r="A12" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="150"/>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="150"/>
-      <c r="F12" s="150"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="147" t="s">
+      <c r="B12" s="155"/>
+      <c r="C12" s="155"/>
+      <c r="D12" s="155"/>
+      <c r="E12" s="155"/>
+      <c r="F12" s="155"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
+      <c r="I12" s="153"/>
+      <c r="J12" s="153"/>
+      <c r="K12" s="153"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="153"/>
+      <c r="N12" s="153"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="133"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="147" t="s">
+      <c r="A13" s="138"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="140"/>
+      <c r="H13" s="152" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
+      <c r="I13" s="153"/>
+      <c r="J13" s="153"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="153"/>
+      <c r="N13" s="153"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="147" t="s">
+      <c r="A14" s="138"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="139"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="148"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="153"/>
+      <c r="N14" s="153"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="147" t="s">
+      <c r="A15" s="138"/>
+      <c r="B15" s="139"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="139"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="140"/>
+      <c r="H15" s="152" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-      <c r="L15" s="148"/>
-      <c r="M15" s="148"/>
-      <c r="N15" s="148"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="153"/>
+      <c r="K15" s="153"/>
+      <c r="L15" s="153"/>
+      <c r="M15" s="153"/>
+      <c r="N15" s="153"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -16586,10 +16997,10 @@
       <c r="C189" s="61">
         <v>2</v>
       </c>
-      <c r="D189" s="152" t="s">
+      <c r="D189" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E189" s="153" t="s">
+      <c r="E189" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G189" s="61">
@@ -16598,10 +17009,10 @@
       <c r="H189" s="61">
         <v>3</v>
       </c>
-      <c r="I189" s="152" t="s">
+      <c r="I189" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J189" s="153" t="s">
+      <c r="J189" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L189" s="61">
@@ -16610,10 +17021,10 @@
       <c r="M189" s="61">
         <v>4</v>
       </c>
-      <c r="N189" s="152" t="s">
+      <c r="N189" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O189" s="153" t="s">
+      <c r="O189" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q189" s="61">
@@ -16622,10 +17033,10 @@
       <c r="R189" s="61">
         <v>5</v>
       </c>
-      <c r="S189" s="152" t="s">
+      <c r="S189" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T189" s="153" t="s">
+      <c r="T189" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16636,10 +17047,10 @@
       <c r="C190" s="61">
         <v>3</v>
       </c>
-      <c r="D190" s="152" t="s">
+      <c r="D190" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E190" s="153" t="s">
+      <c r="E190" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G190" s="61">
@@ -16648,10 +17059,10 @@
       <c r="H190" s="61">
         <v>4</v>
       </c>
-      <c r="I190" s="152" t="s">
+      <c r="I190" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J190" s="153" t="s">
+      <c r="J190" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L190" s="61">
@@ -16660,10 +17071,10 @@
       <c r="M190" s="61">
         <v>5</v>
       </c>
-      <c r="N190" s="152" t="s">
+      <c r="N190" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O190" s="153" t="s">
+      <c r="O190" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q190" s="61">
@@ -16672,10 +17083,10 @@
       <c r="R190" s="61">
         <v>6</v>
       </c>
-      <c r="S190" s="152" t="s">
+      <c r="S190" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T190" s="153" t="s">
+      <c r="T190" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16686,10 +17097,10 @@
       <c r="C191" s="61">
         <v>4</v>
       </c>
-      <c r="D191" s="152" t="s">
+      <c r="D191" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E191" s="153" t="s">
+      <c r="E191" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G191" s="61">
@@ -16698,10 +17109,10 @@
       <c r="H191" s="61">
         <v>5</v>
       </c>
-      <c r="I191" s="152" t="s">
+      <c r="I191" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J191" s="153" t="s">
+      <c r="J191" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L191" s="61">
@@ -16710,10 +17121,10 @@
       <c r="M191" s="61">
         <v>6</v>
       </c>
-      <c r="N191" s="152" t="s">
+      <c r="N191" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O191" s="153" t="s">
+      <c r="O191" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q191" s="61">
@@ -16722,10 +17133,10 @@
       <c r="R191" s="61">
         <v>7</v>
       </c>
-      <c r="S191" s="152" t="s">
+      <c r="S191" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T191" s="153" t="s">
+      <c r="T191" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16736,10 +17147,10 @@
       <c r="C192" s="61">
         <v>5</v>
       </c>
-      <c r="D192" s="152" t="s">
+      <c r="D192" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E192" s="153" t="s">
+      <c r="E192" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G192" s="61">
@@ -16748,10 +17159,10 @@
       <c r="H192" s="61">
         <v>6</v>
       </c>
-      <c r="I192" s="152" t="s">
+      <c r="I192" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J192" s="153" t="s">
+      <c r="J192" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L192" s="61">
@@ -16760,10 +17171,10 @@
       <c r="M192" s="61">
         <v>7</v>
       </c>
-      <c r="N192" s="152" t="s">
+      <c r="N192" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O192" s="153" t="s">
+      <c r="O192" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q192" s="61">
@@ -16772,10 +17183,10 @@
       <c r="R192" s="61">
         <v>8</v>
       </c>
-      <c r="S192" s="152" t="s">
+      <c r="S192" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T192" s="153" t="s">
+      <c r="T192" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16786,10 +17197,10 @@
       <c r="C193" s="61">
         <v>6</v>
       </c>
-      <c r="D193" s="152" t="s">
+      <c r="D193" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E193" s="153" t="s">
+      <c r="E193" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G193" s="61">
@@ -16798,10 +17209,10 @@
       <c r="H193" s="61">
         <v>7</v>
       </c>
-      <c r="I193" s="152" t="s">
+      <c r="I193" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J193" s="153" t="s">
+      <c r="J193" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L193" s="61">
@@ -16810,10 +17221,10 @@
       <c r="M193" s="61">
         <v>8</v>
       </c>
-      <c r="N193" s="152" t="s">
+      <c r="N193" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O193" s="153" t="s">
+      <c r="O193" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q193" s="61">
@@ -16822,10 +17233,10 @@
       <c r="R193" s="61">
         <v>101</v>
       </c>
-      <c r="S193" s="152" t="s">
+      <c r="S193" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T193" s="153" t="s">
+      <c r="T193" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16836,10 +17247,10 @@
       <c r="C194" s="61">
         <v>7</v>
       </c>
-      <c r="D194" s="152" t="s">
+      <c r="D194" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E194" s="153" t="s">
+      <c r="E194" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G194" s="61">
@@ -16848,10 +17259,10 @@
       <c r="H194" s="61">
         <v>8</v>
       </c>
-      <c r="I194" s="152" t="s">
+      <c r="I194" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J194" s="153" t="s">
+      <c r="J194" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L194" s="61">
@@ -16860,10 +17271,10 @@
       <c r="M194" s="61">
         <v>101</v>
       </c>
-      <c r="N194" s="152" t="s">
+      <c r="N194" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O194" s="153" t="s">
+      <c r="O194" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q194" s="61">
@@ -16872,10 +17283,10 @@
       <c r="R194" s="61">
         <v>102</v>
       </c>
-      <c r="S194" s="152" t="s">
+      <c r="S194" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T194" s="152" t="s">
+      <c r="T194" s="114" t="s">
         <v>327</v>
       </c>
     </row>
@@ -16886,10 +17297,10 @@
       <c r="C195" s="61">
         <v>8</v>
       </c>
-      <c r="D195" s="152" t="s">
+      <c r="D195" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E195" s="153" t="s">
+      <c r="E195" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G195" s="61">
@@ -16898,10 +17309,10 @@
       <c r="H195" s="61">
         <v>101</v>
       </c>
-      <c r="I195" s="152" t="s">
+      <c r="I195" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J195" s="152" t="s">
+      <c r="J195" s="114" t="s">
         <v>327</v>
       </c>
       <c r="L195" s="61">
@@ -16910,10 +17321,10 @@
       <c r="M195" s="61">
         <v>102</v>
       </c>
-      <c r="N195" s="152" t="s">
+      <c r="N195" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O195" s="153" t="s">
+      <c r="O195" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q195" s="61">
@@ -16922,10 +17333,10 @@
       <c r="R195" s="61">
         <v>103</v>
       </c>
-      <c r="S195" s="152" t="s">
+      <c r="S195" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T195" s="153" t="s">
+      <c r="T195" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16936,10 +17347,10 @@
       <c r="C196" s="61">
         <v>101</v>
       </c>
-      <c r="D196" s="152" t="s">
+      <c r="D196" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E196" s="153" t="s">
+      <c r="E196" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G196" s="61">
@@ -16948,10 +17359,10 @@
       <c r="H196" s="61">
         <v>102</v>
       </c>
-      <c r="I196" s="152" t="s">
+      <c r="I196" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J196" s="153" t="s">
+      <c r="J196" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L196" s="61">
@@ -16960,10 +17371,10 @@
       <c r="M196" s="61">
         <v>103</v>
       </c>
-      <c r="N196" s="152" t="s">
+      <c r="N196" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O196" s="153" t="s">
+      <c r="O196" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -16974,10 +17385,10 @@
       <c r="C197" s="61">
         <v>102</v>
       </c>
-      <c r="D197" s="152" t="s">
+      <c r="D197" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E197" s="153" t="s">
+      <c r="E197" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G197" s="61">
@@ -16986,10 +17397,10 @@
       <c r="H197" s="61">
         <v>103</v>
       </c>
-      <c r="I197" s="152" t="s">
+      <c r="I197" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J197" s="153" t="s">
+      <c r="J197" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17000,10 +17411,10 @@
       <c r="C198" s="61">
         <v>103</v>
       </c>
-      <c r="D198" s="152" t="s">
+      <c r="D198" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E198" s="153" t="s">
+      <c r="E198" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17108,10 +17519,10 @@
       <c r="C204" s="61">
         <v>6</v>
       </c>
-      <c r="D204" s="152" t="s">
+      <c r="D204" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E204" s="153" t="s">
+      <c r="E204" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G204" s="61">
@@ -17120,10 +17531,10 @@
       <c r="H204" s="61">
         <v>7</v>
       </c>
-      <c r="I204" s="152" t="s">
+      <c r="I204" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J204" s="153" t="s">
+      <c r="J204" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L204" s="61">
@@ -17132,10 +17543,10 @@
       <c r="M204" s="61">
         <v>8</v>
       </c>
-      <c r="N204" s="152" t="s">
+      <c r="N204" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O204" s="153" t="s">
+      <c r="O204" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q204" s="61">
@@ -17144,10 +17555,10 @@
       <c r="R204" s="61">
         <v>101</v>
       </c>
-      <c r="S204" s="152" t="s">
+      <c r="S204" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T204" s="153" t="s">
+      <c r="T204" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17158,10 +17569,10 @@
       <c r="C205" s="61">
         <v>7</v>
       </c>
-      <c r="D205" s="152" t="s">
+      <c r="D205" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E205" s="153" t="s">
+      <c r="E205" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G205" s="61">
@@ -17170,10 +17581,10 @@
       <c r="H205" s="61">
         <v>8</v>
       </c>
-      <c r="I205" s="152" t="s">
+      <c r="I205" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J205" s="153" t="s">
+      <c r="J205" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L205" s="61">
@@ -17182,10 +17593,10 @@
       <c r="M205" s="61">
         <v>101</v>
       </c>
-      <c r="N205" s="152" t="s">
+      <c r="N205" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O205" s="153" t="s">
+      <c r="O205" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q205" s="61">
@@ -17194,10 +17605,10 @@
       <c r="R205" s="61">
         <v>102</v>
       </c>
-      <c r="S205" s="152" t="s">
+      <c r="S205" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T205" s="153" t="s">
+      <c r="T205" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17208,10 +17619,10 @@
       <c r="C206" s="61">
         <v>8</v>
       </c>
-      <c r="D206" s="152" t="s">
+      <c r="D206" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E206" s="153" t="s">
+      <c r="E206" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G206" s="61">
@@ -17220,10 +17631,10 @@
       <c r="H206" s="61">
         <v>101</v>
       </c>
-      <c r="I206" s="152" t="s">
+      <c r="I206" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J206" s="153" t="s">
+      <c r="J206" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L206" s="61">
@@ -17232,10 +17643,10 @@
       <c r="M206" s="61">
         <v>102</v>
       </c>
-      <c r="N206" s="152" t="s">
+      <c r="N206" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O206" s="153" t="s">
+      <c r="O206" s="115" t="s">
         <v>328</v>
       </c>
       <c r="Q206" s="61">
@@ -17244,10 +17655,10 @@
       <c r="R206" s="61">
         <v>103</v>
       </c>
-      <c r="S206" s="152" t="s">
+      <c r="S206" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="T206" s="153" t="s">
+      <c r="T206" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17258,10 +17669,10 @@
       <c r="C207" s="61">
         <v>101</v>
       </c>
-      <c r="D207" s="152" t="s">
+      <c r="D207" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E207" s="153" t="s">
+      <c r="E207" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G207" s="61">
@@ -17270,10 +17681,10 @@
       <c r="H207" s="61">
         <v>102</v>
       </c>
-      <c r="I207" s="152" t="s">
+      <c r="I207" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J207" s="153" t="s">
+      <c r="J207" s="115" t="s">
         <v>328</v>
       </c>
       <c r="L207" s="61">
@@ -17282,10 +17693,10 @@
       <c r="M207" s="61">
         <v>103</v>
       </c>
-      <c r="N207" s="152" t="s">
+      <c r="N207" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="O207" s="153" t="s">
+      <c r="O207" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17296,10 +17707,10 @@
       <c r="C208" s="61">
         <v>102</v>
       </c>
-      <c r="D208" s="152" t="s">
+      <c r="D208" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E208" s="153" t="s">
+      <c r="E208" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G208" s="61">
@@ -17308,10 +17719,10 @@
       <c r="H208" s="61">
         <v>103</v>
       </c>
-      <c r="I208" s="152" t="s">
+      <c r="I208" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J208" s="153" t="s">
+      <c r="J208" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17322,10 +17733,10 @@
       <c r="C209" s="61">
         <v>103</v>
       </c>
-      <c r="D209" s="152" t="s">
+      <c r="D209" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E209" s="152" t="s">
+      <c r="E209" s="114" t="s">
         <v>327</v>
       </c>
     </row>
@@ -17386,10 +17797,10 @@
       <c r="C215" s="61">
         <v>102</v>
       </c>
-      <c r="D215" s="152" t="s">
+      <c r="D215" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E215" s="153" t="s">
+      <c r="E215" s="115" t="s">
         <v>328</v>
       </c>
       <c r="G215" s="61">
@@ -17398,10 +17809,10 @@
       <c r="H215" s="61">
         <v>103</v>
       </c>
-      <c r="I215" s="152" t="s">
+      <c r="I215" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="J215" s="153" t="s">
+      <c r="J215" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17412,10 +17823,10 @@
       <c r="C216" s="61">
         <v>103</v>
       </c>
-      <c r="D216" s="152" t="s">
+      <c r="D216" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E216" s="153" t="s">
+      <c r="E216" s="115" t="s">
         <v>328</v>
       </c>
     </row>
@@ -17454,10 +17865,10 @@
       <c r="C222" s="61">
         <v>101</v>
       </c>
-      <c r="D222" s="152" t="s">
+      <c r="D222" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E222" s="152" t="s">
+      <c r="E222" s="114" t="s">
         <v>327</v>
       </c>
     </row>
@@ -17474,10 +17885,10 @@
       <c r="C224" s="61">
         <v>102</v>
       </c>
-      <c r="D224" s="152" t="s">
+      <c r="D224" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E224" s="152" t="s">
+      <c r="E224" s="114" t="s">
         <v>327</v>
       </c>
     </row>
@@ -17494,10 +17905,10 @@
       <c r="C226" s="61">
         <v>103</v>
       </c>
-      <c r="D226" s="152" t="s">
+      <c r="D226" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="E226" s="152" t="s">
+      <c r="E226" s="114" t="s">
         <v>327</v>
       </c>
     </row>
@@ -18588,7 +18999,7 @@
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" s="91"/>
-      <c r="B378" s="154"/>
+      <c r="B378" s="116"/>
       <c r="C378" s="91"/>
       <c r="D378" s="91"/>
       <c r="E378" s="91"/>
@@ -18600,7 +19011,7 @@
     <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379" s="91"/>
       <c r="B379" s="91"/>
-      <c r="C379" s="155"/>
+      <c r="C379" s="117"/>
       <c r="D379" s="91"/>
       <c r="E379" s="91"/>
       <c r="F379" s="91"/>
@@ -18666,7 +19077,7 @@
     <row r="385" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A385" s="91"/>
       <c r="B385" s="91"/>
-      <c r="C385" s="156"/>
+      <c r="C385" s="118"/>
       <c r="D385" s="91"/>
       <c r="E385" s="91"/>
       <c r="F385" s="91"/>
@@ -18709,6 +19120,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="H10:N10"/>
+    <mergeCell ref="H7:N7"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="H15:N15"/>
     <mergeCell ref="A12:G12"/>
@@ -18717,13 +19135,6 @@
     <mergeCell ref="H13:N13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="H14:N14"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="H7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18798,24 +19209,24 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="149" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151" t="s">
         <v>119</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
       <c r="Q6" s="66"/>
       <c r="S6" s="67"/>
     </row>
@@ -18827,15 +19238,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="151" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
       <c r="Q7" s="66"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -18843,24 +19254,24 @@
       <c r="S8" s="68"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="141" t="s">
+      <c r="A9" s="149" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="117"/>
-      <c r="C9" s="117"/>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="147" t="s">
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="150"/>
+      <c r="H9" s="152" t="s">
         <v>122</v>
       </c>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="153"/>
+      <c r="K9" s="153"/>
+      <c r="L9" s="153"/>
+      <c r="M9" s="153"/>
+      <c r="N9" s="153"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -18870,15 +19281,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="143" t="s">
+      <c r="H10" s="151" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="148"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="153"/>
+      <c r="K10" s="153"/>
+      <c r="L10" s="153"/>
+      <c r="M10" s="153"/>
+      <c r="N10" s="153"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
@@ -18888,33 +19299,33 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="143" t="s">
+      <c r="H11" s="151" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="147" t="s">
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="152" t="s">
         <v>126</v>
       </c>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
+      <c r="I12" s="153"/>
+      <c r="J12" s="153"/>
+      <c r="K12" s="153"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="153"/>
+      <c r="N12" s="153"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -18924,15 +19335,15 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="143" t="s">
+      <c r="H13" s="151" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
+      <c r="I13" s="153"/>
+      <c r="J13" s="153"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="153"/>
+      <c r="N13" s="153"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
@@ -18942,15 +19353,15 @@
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="143" t="s">
+      <c r="H14" s="151" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="148"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="153"/>
+      <c r="N14" s="153"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
@@ -18960,15 +19371,15 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="143" t="s">
+      <c r="H15" s="151" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-      <c r="L15" s="148"/>
-      <c r="M15" s="148"/>
-      <c r="N15" s="148"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="153"/>
+      <c r="K15" s="153"/>
+      <c r="L15" s="153"/>
+      <c r="M15" s="153"/>
+      <c r="N15" s="153"/>
       <c r="T15" s="69"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -18979,15 +19390,15 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="143" t="s">
+      <c r="H16" s="151" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="148"/>
-      <c r="L16" s="148"/>
-      <c r="M16" s="148"/>
-      <c r="N16" s="148"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
+      <c r="K16" s="153"/>
+      <c r="L16" s="153"/>
+      <c r="M16" s="153"/>
+      <c r="N16" s="153"/>
       <c r="T16" s="68"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -18998,15 +19409,15 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
-      <c r="H17" s="143" t="s">
+      <c r="H17" s="151" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="148"/>
-      <c r="J17" s="148"/>
-      <c r="K17" s="148"/>
-      <c r="L17" s="148"/>
-      <c r="M17" s="148"/>
-      <c r="N17" s="148"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="153"/>
+      <c r="K17" s="153"/>
+      <c r="L17" s="153"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="153"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
@@ -19016,15 +19427,15 @@
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-      <c r="H18" s="143" t="s">
+      <c r="H18" s="151" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="148"/>
-      <c r="J18" s="148"/>
-      <c r="K18" s="148"/>
-      <c r="L18" s="148"/>
-      <c r="M18" s="148"/>
-      <c r="N18" s="148"/>
+      <c r="I18" s="153"/>
+      <c r="J18" s="153"/>
+      <c r="K18" s="153"/>
+      <c r="L18" s="153"/>
+      <c r="M18" s="153"/>
+      <c r="N18" s="153"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T19" s="69"/>
@@ -20336,24 +20747,24 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="149" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
       <c r="Q6" s="66"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -20364,15 +20775,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
       <c r="Q7" s="66"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -20383,15 +20794,15 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="143" t="s">
+      <c r="H8" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="124"/>
+      <c r="N8" s="124"/>
       <c r="Q8" s="66"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20402,15 +20813,15 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="143" t="s">
+      <c r="H9" s="151" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
       <c r="Q9" s="66"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20421,15 +20832,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="143" t="s">
+      <c r="H10" s="151" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="124"/>
       <c r="Q10" s="66"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20440,15 +20851,15 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="143" t="s">
+      <c r="H11" s="151" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
       <c r="Q11" s="66"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20459,15 +20870,15 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="143" t="s">
+      <c r="H12" s="151" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="124"/>
+      <c r="M12" s="124"/>
+      <c r="N12" s="124"/>
       <c r="Q12" s="66"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20478,15 +20889,15 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="143" t="s">
+      <c r="H13" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
       <c r="Q13" s="66"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20497,15 +20908,15 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="143" t="s">
+      <c r="H14" s="151" t="s">
         <v>135</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
       <c r="Q14" s="66"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20516,15 +20927,15 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="143" t="s">
+      <c r="H15" s="151" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
       <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -21877,24 +22288,24 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="149" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="151" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
       <c r="Q6" s="66"/>
       <c r="R6" s="69"/>
       <c r="S6" s="68"/>
@@ -21908,15 +22319,15 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="143" t="s">
+      <c r="H7" s="151" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
       <c r="Q7" s="66"/>
       <c r="R7" s="69"/>
       <c r="S7" s="68"/>
@@ -21930,15 +22341,15 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="143" t="s">
+      <c r="H8" s="151" t="s">
         <v>148</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="124"/>
+      <c r="N8" s="124"/>
       <c r="Q8" s="66"/>
       <c r="R8" s="69"/>
       <c r="S8" s="68"/>
@@ -21952,15 +22363,15 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="143" t="s">
+      <c r="H9" s="151" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
       <c r="Q9" s="66"/>
       <c r="R9" s="69"/>
       <c r="S9" s="68"/>
@@ -21974,15 +22385,15 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="143" t="s">
+      <c r="H10" s="151" t="s">
         <v>150</v>
       </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="124"/>
       <c r="Q10" s="66"/>
       <c r="R10" s="69"/>
       <c r="S10" s="68"/>
@@ -21996,13 +22407,13 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
       <c r="Q11" s="66"/>
       <c r="R11" s="69"/>
       <c r="S11" s="69"/>
@@ -22016,15 +22427,15 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="143" t="s">
+      <c r="H12" s="151" t="s">
         <v>151</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="124"/>
+      <c r="M12" s="124"/>
+      <c r="N12" s="124"/>
       <c r="Q12" s="66"/>
       <c r="S12" s="69"/>
     </row>
@@ -22036,15 +22447,15 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="143" t="s">
+      <c r="H13" s="151" t="s">
         <v>152</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="124"/>
       <c r="Q13" s="66"/>
       <c r="S13" s="69"/>
     </row>
@@ -22056,15 +22467,15 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="143" t="s">
+      <c r="H14" s="151" t="s">
         <v>144</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
       <c r="Q14" s="66"/>
       <c r="S14" s="69"/>
     </row>
@@ -22076,15 +22487,15 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="143" t="s">
+      <c r="H15" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
       <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -23398,17 +23809,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="H15:N15"/>
     <mergeCell ref="H10:N10"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:N6"/>
     <mergeCell ref="H7:N7"/>
     <mergeCell ref="H8:N8"/>
     <mergeCell ref="H9:N9"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="H15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -25184,8 +25595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED752DCA-8D76-432A-A777-3706FAB32113}">
   <dimension ref="B1:U215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="P217" sqref="P217"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27765,8 +28176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433504EA-A577-465B-995B-20D09D833E52}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27778,6 +28189,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27785,7 +28197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F21AE47-F189-47C6-8FE5-A7A33F4788D5}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -27796,6 +28210,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27998,24 +28413,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -28397,44 +28812,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="118" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -28698,44 +29113,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="118" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -29008,24 +29423,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -29115,24 +29530,24 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -29245,64 +29660,64 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="118" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
     </row>
     <row r="8" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="118" t="s">
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="124"/>
+      <c r="N8" s="124"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -29684,44 +30099,44 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="118" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="118" t="s">
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>